<commit_message>
First batch of bug fixes
</commit_message>
<xml_diff>
--- a/317 Newell St/Results/Excels/Exec_Summary_Performance_KPIs.xlsx
+++ b/317 Newell St/Results/Excels/Exec_Summary_Performance_KPIs.xlsx
@@ -82,7 +82,7 @@
     <t>$12833.33</t>
   </si>
   <si>
-    <t>$-4041.69</t>
+    <t>$-3963.69</t>
   </si>
   <si>
     <t>$37328.35</t>
@@ -91,16 +91,16 @@
     <t>$43862.50</t>
   </si>
   <si>
-    <t>$21686.66</t>
-  </si>
-  <si>
-    <t>-9.14%</t>
+    <t>$21764.66</t>
+  </si>
+  <si>
+    <t>-9.04%</t>
   </si>
   <si>
     <t>-100.00%</t>
   </si>
   <si>
-    <t>3.28%</t>
+    <t>3.33%</t>
   </si>
   <si>
     <t>8.85%</t>
@@ -109,22 +109,22 @@
     <t>$15785.00</t>
   </si>
   <si>
-    <t>$-1836.28</t>
+    <t>$-1614.28</t>
   </si>
   <si>
     <t>$41386.10</t>
   </si>
   <si>
-    <t>$23676.13</t>
-  </si>
-  <si>
-    <t>-3.90%</t>
-  </si>
-  <si>
-    <t>-46.02%</t>
-  </si>
-  <si>
-    <t>4.80%</t>
+    <t>$23976.13</t>
+  </si>
+  <si>
+    <t>-3.68%</t>
+  </si>
+  <si>
+    <t>-45.34%</t>
+  </si>
+  <si>
+    <t>4.95%</t>
   </si>
   <si>
     <t>10.89%</t>
@@ -133,22 +133,22 @@
     <t>$16179.62</t>
   </si>
   <si>
-    <t>$-1808.63</t>
+    <t>$-1442.63</t>
   </si>
   <si>
     <t>$45587.08</t>
   </si>
   <si>
-    <t>$25831.84</t>
-  </si>
-  <si>
-    <t>-4.13%</t>
-  </si>
-  <si>
-    <t>-23.26%</t>
-  </si>
-  <si>
-    <t>4.82%</t>
+    <t>$26497.84</t>
+  </si>
+  <si>
+    <t>-3.29%</t>
+  </si>
+  <si>
+    <t>-22.28%</t>
+  </si>
+  <si>
+    <t>5.07%</t>
   </si>
   <si>
     <t>11.16%</t>
@@ -157,22 +157,22 @@
     <t>$16584.12</t>
   </si>
   <si>
-    <t>$-1777.01</t>
+    <t>$-1267.01</t>
   </si>
   <si>
     <t>$49938.73</t>
   </si>
   <si>
-    <t>$28165.11</t>
-  </si>
-  <si>
-    <t>-4.06%</t>
-  </si>
-  <si>
-    <t>-13.73%</t>
-  </si>
-  <si>
-    <t>4.84%</t>
+    <t>$29341.11</t>
+  </si>
+  <si>
+    <t>-2.89%</t>
+  </si>
+  <si>
+    <t>-12.54%</t>
+  </si>
+  <si>
+    <t>5.19%</t>
   </si>
   <si>
     <t>11.44%</t>
@@ -181,22 +181,22 @@
     <t>$16998.72</t>
   </si>
   <si>
-    <t>$-1741.32</t>
+    <t>$-1087.32</t>
   </si>
   <si>
     <t>$54448.98</t>
   </si>
   <si>
-    <t>$30687.83</t>
-  </si>
-  <si>
-    <t>-3.98%</t>
-  </si>
-  <si>
-    <t>-8.54%</t>
-  </si>
-  <si>
-    <t>4.86%</t>
+    <t>$32517.83</t>
+  </si>
+  <si>
+    <t>-2.48%</t>
+  </si>
+  <si>
+    <t>-7.21%</t>
+  </si>
+  <si>
+    <t>5.31%</t>
   </si>
   <si>
     <t>11.72%</t>
@@ -205,22 +205,22 @@
     <t>$17423.69</t>
   </si>
   <si>
-    <t>$-1701.48</t>
+    <t>$-903.48</t>
   </si>
   <si>
     <t>$59126.26</t>
   </si>
   <si>
-    <t>$33412.51</t>
-  </si>
-  <si>
-    <t>-3.89%</t>
-  </si>
-  <si>
-    <t>-5.30%</t>
-  </si>
-  <si>
-    <t>4.89%</t>
+    <t>$36040.51</t>
+  </si>
+  <si>
+    <t>-2.06%</t>
+  </si>
+  <si>
+    <t>-3.85%</t>
+  </si>
+  <si>
+    <t>5.44%</t>
   </si>
   <si>
     <t>12.02%</t>
@@ -229,22 +229,22 @@
     <t>$17859.28</t>
   </si>
   <si>
-    <t>$-1657.39</t>
+    <t>$-715.39</t>
   </si>
   <si>
     <t>$63979.57</t>
   </si>
   <si>
-    <t>$36352.29</t>
-  </si>
-  <si>
-    <t>-3.79%</t>
-  </si>
-  <si>
-    <t>-3.08%</t>
-  </si>
-  <si>
-    <t>4.92%</t>
+    <t>$39922.29</t>
+  </si>
+  <si>
+    <t>-1.63%</t>
+  </si>
+  <si>
+    <t>-1.56%</t>
+  </si>
+  <si>
+    <t>5.57%</t>
   </si>
   <si>
     <t>12.32%</t>
@@ -253,22 +253,22 @@
     <t>$18305.76</t>
   </si>
   <si>
-    <t>$-1608.96</t>
+    <t>$-522.96</t>
   </si>
   <si>
     <t>$69018.51</t>
   </si>
   <si>
-    <t>$39520.99</t>
-  </si>
-  <si>
-    <t>-3.68%</t>
-  </si>
-  <si>
-    <t>-1.48%</t>
-  </si>
-  <si>
-    <t>4.95%</t>
+    <t>$44176.99</t>
+  </si>
+  <si>
+    <t>-1.19%</t>
+  </si>
+  <si>
+    <t>0.10%</t>
+  </si>
+  <si>
+    <t>5.70%</t>
   </si>
   <si>
     <t>12.62%</t>
@@ -277,22 +277,22 @@
     <t>$18763.40</t>
   </si>
   <si>
-    <t>$-1556.11</t>
+    <t>$-326.11</t>
   </si>
   <si>
     <t>$74253.30</t>
   </si>
   <si>
-    <t>$42933.18</t>
-  </si>
-  <si>
-    <t>-3.56%</t>
-  </si>
-  <si>
-    <t>-0.27%</t>
-  </si>
-  <si>
-    <t>4.99%</t>
+    <t>$48819.18</t>
+  </si>
+  <si>
+    <t>-0.74%</t>
+  </si>
+  <si>
+    <t>1.35%</t>
+  </si>
+  <si>
+    <t>5.84%</t>
   </si>
   <si>
     <t>12.94%</t>
@@ -301,22 +301,22 @@
     <t>$19232.49</t>
   </si>
   <si>
-    <t>$-1498.72</t>
+    <t>$-124.72</t>
   </si>
   <si>
     <t>$79694.87</t>
   </si>
   <si>
-    <t>$46604.20</t>
-  </si>
-  <si>
-    <t>-3.43%</t>
-  </si>
-  <si>
-    <t>0.68%</t>
-  </si>
-  <si>
-    <t>5.03%</t>
+    <t>$53864.20</t>
+  </si>
+  <si>
+    <t>-0.28%</t>
+  </si>
+  <si>
+    <t>2.31%</t>
+  </si>
+  <si>
+    <t>5.98%</t>
   </si>
   <si>
     <t>13.26%</t>
@@ -1038,31 +1038,31 @@
         <v>1.31</v>
       </c>
       <c r="C11">
-        <v>1.12</v>
+        <v>1.1</v>
       </c>
       <c r="D11">
-        <v>1.11</v>
+        <v>1.09</v>
       </c>
       <c r="E11">
-        <v>1.11</v>
+        <v>1.08</v>
       </c>
       <c r="F11">
-        <v>1.1</v>
+        <v>1.06</v>
       </c>
       <c r="G11">
-        <v>1.1</v>
+        <v>1.05</v>
       </c>
       <c r="H11">
-        <v>1.09</v>
+        <v>1.04</v>
       </c>
       <c r="I11">
-        <v>1.09</v>
+        <v>1.03</v>
       </c>
       <c r="J11">
-        <v>1.08</v>
+        <v>1.02</v>
       </c>
       <c r="K11">
-        <v>1.08</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="12" spans="1:11">

</xml_diff>